<commit_message>
Added save generated report test case
</commit_message>
<xml_diff>
--- a/Documents/FINAL/sprint4testReport.xlsx
+++ b/Documents/FINAL/sprint4testReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Sub Levels</t>
   </si>
@@ -52,10 +52,22 @@
     <t>Generate report</t>
   </si>
   <si>
-    <t>T_C_</t>
-  </si>
-  <si>
     <t>Save generated report</t>
+  </si>
+  <si>
+    <t>T_C_105.1</t>
+  </si>
+  <si>
+    <t>T_C_105.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report button is clicked before any cultivation </t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>T_C_105.3</t>
   </si>
 </sst>
 </file>
@@ -196,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -233,6 +245,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +588,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>11</v>
@@ -642,10 +655,12 @@
     </row>
     <row r="3" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>
@@ -661,14 +676,36 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="14">
+        <v>42747</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6"/>

</xml_diff>

<commit_message>
Final Sprint Planning Document, FinalProject Plan Completed
</commit_message>
<xml_diff>
--- a/Documents/FINAL/sprint4testReport.xlsx
+++ b/Documents/FINAL/sprint4testReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Sub Levels</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>Save generated report</t>
+  </si>
+  <si>
+    <t>Save Report</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -575,22 +581,22 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="48.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -616,7 +622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -634,105 +640,111 @@
         <v>6</v>
       </c>
       <c r="G2" s="7">
-        <v>42746</v>
+        <v>42752</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+    <row r="3" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="7">
-        <v>42746</v>
+        <v>42752</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F9"/>
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="6:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="6:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="6:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="6:8" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="6:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="6:8" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>